<commit_message>
added PCA / SHP
</commit_message>
<xml_diff>
--- a/doclib/Referencias.xlsx
+++ b/doclib/Referencias.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/99c71d5d6f66413c/Python/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/99c71d5d6f66413c/Python/ia_ml/doclib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="11_684457EADBE0FBDD3A0AC92861C12AAD415917E1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05D90A9E-7C5B-4E6E-A3BD-70005382A460}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="11_684457EADBE0FBDD3A0AC92861C12AAD415917E1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F51B486-AC84-48AD-AFB4-6CA78539876A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
   <si>
     <t>Numpy</t>
   </si>
@@ -799,6 +799,127 @@
   </si>
   <si>
     <t>Rotacao: a variancia total e comonalidades não muda, somente a distribuição</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>autovalores</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> indicam o percentual da variância compartilhada pelas variáveis originais para a formação de cada fator</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Scores fatoriais</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: são os parâmetros que relacionam o fator com as variáveis originais, representados em um modelo linear</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>As</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cargas fatoriais </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>representam as correlações de Pearson entre os fatores e as variáveis originais. Pode ser interpretada como a importância de cada variável na constituição daquele fator. Quanto maior a carga fatorial, mais aquele fator é influenciado pela variável</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>comunalidades</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> mostram a variância total compartilhada, para cada variável, em todos os fatores extraídos e selecionados. É possível analisar se houve perda de variância, por variável, </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Para criar </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rankings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> a partir dos fatores obtidos , multiplica-se o resultado obtido de cada fator por seu percentual de variância compartilhada e depois é realizado o ordenamento do resultado</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -923,7 +1044,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -970,6 +1091,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1176,13 +1300,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>5176134</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>172202</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1220,13 +1344,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>5495925</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>544051</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>184260</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2044,10 +2168,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9065BC9-6437-4A90-8675-040CA624184B}">
-  <dimension ref="B2:C11"/>
+  <dimension ref="B2:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,51 +2180,69 @@
     <col min="3" max="3" width="94.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>101</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="C6" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
-      <c r="C7" s="6" t="s">
+    <row r="9" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="17"/>
+      <c r="C9" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+    <row r="13" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
         <v>105</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update documentation and add PCA/ANACOR
</commit_message>
<xml_diff>
--- a/doclib/Referencias.xlsx
+++ b/doclib/Referencias.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/99c71d5d6f66413c/Python/ia_ml/doclib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="11_684457EADBE0FBDD3A0AC92861C12AAD415917E1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F51B486-AC84-48AD-AFB4-6CA78539876A}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="11_684457EADBE0FBDD3A0AC92861C12AAD415917E1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87EDEB63-B7A4-48D5-A4F7-5FBDD49FA91B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="EngDados" sheetId="8" r:id="rId1"/>
-    <sheet name="bibliotecas" sheetId="1" r:id="rId2"/>
-    <sheet name="CLustering" sheetId="4" r:id="rId3"/>
-    <sheet name="AnaliseFatorial" sheetId="10" r:id="rId4"/>
-    <sheet name="Classificação" sheetId="2" r:id="rId5"/>
-    <sheet name="Pre-Processamento" sheetId="9" r:id="rId6"/>
-    <sheet name="Regressão" sheetId="3" r:id="rId7"/>
-    <sheet name="ClustersValidacao" sheetId="5" r:id="rId8"/>
-    <sheet name="Ferramentas" sheetId="6" r:id="rId9"/>
-    <sheet name="Regressao Linear" sheetId="7" r:id="rId10"/>
+    <sheet name="BIG Picture ML" sheetId="12" r:id="rId1"/>
+    <sheet name="CLustering" sheetId="4" r:id="rId2"/>
+    <sheet name="PCA" sheetId="10" r:id="rId3"/>
+    <sheet name="ANACOR" sheetId="11" r:id="rId4"/>
+    <sheet name="bibliotecas" sheetId="1" r:id="rId5"/>
+    <sheet name="Classificação" sheetId="2" r:id="rId6"/>
+    <sheet name="Pre-Processamento" sheetId="9" r:id="rId7"/>
+    <sheet name="Regressão" sheetId="3" r:id="rId8"/>
+    <sheet name="ClustersValidacao" sheetId="5" r:id="rId9"/>
+    <sheet name="Ferramentas" sheetId="6" r:id="rId10"/>
+    <sheet name="Regressao Linear" sheetId="7" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="149">
   <si>
     <t>Numpy</t>
   </si>
@@ -541,15 +542,6 @@
       </rPr>
       <t>: também conhecidos por "coeficientes parciais de regressão" ou "coeficientes parciais angulares". É obtido por meio do valor médio de Y, com a variação de uma unidade de uma determinada variável X.  modelo.coef_</t>
     </r>
-  </si>
-  <si>
-    <t>Spark</t>
-  </si>
-  <si>
-    <t>Airflow</t>
-  </si>
-  <si>
-    <t>Apache Beans</t>
   </si>
   <si>
     <r>
@@ -921,12 +913,182 @@
       <t xml:space="preserve"> a partir dos fatores obtidos , multiplica-se o resultado obtido de cada fator por seu percentual de variância compartilhada e depois é realizado o ordenamento do resultado</t>
     </r>
   </si>
+  <si>
+    <t>Técnica adequada para a análise de variáveis categóricas (qualitativas) para verificar se existe associação estatisticamente significativa entre as variáveis e suas categorias, criando o mapa perceptual para visualizar as associações</t>
+  </si>
+  <si>
+    <t>Caso exista uma variável quantitativa, é necessário que ela passe por um processo de categorização previamente</t>
+  </si>
+  <si>
+    <t>2. Elaboração e interpretação do mapa perceptual</t>
+  </si>
+  <si>
+    <t>1. Análise da significância estatística da associação entre as variáveis e suas categorias por meio do teste qui-quadrado (χ2)</t>
+  </si>
+  <si>
+    <t>Usa a soma do χ2)
+• H0: as variáveis se associam de forma aleatória.
+• H1: a associação entre as variáveis não se dá de forma aleatória.
+• Dados o nível de significância e os graus de liberdade, se o valor da estatística χ2 for maior do que seu valor crítico, há associação significante entre as duas variáveis (H1)
+• Graus de liberdade = (I – 1) x (J – 1)</t>
+  </si>
+  <si>
+    <t>autovalores referem-se às inércias principais parciais e são base para determinar a inércia principal total e o percentual da inércia principal total em cada dimensão do mapa perceptual</t>
+  </si>
+  <si>
+    <t>Autovalores</t>
+  </si>
+  <si>
+    <t>quantidade (m) de autovalores depende da quantidade de categorias nas
+variáveis: m = mín(I – 1, J – 1)</t>
+  </si>
+  <si>
+    <t>As massas representam a influência que cada categoria exerce sobre as demais
+categorias de sua variável</t>
+  </si>
+  <si>
+    <t>Massas das variáveis</t>
+  </si>
+  <si>
+    <t>Autovetores</t>
+  </si>
+  <si>
+    <t>Coordenadas das categorias</t>
+  </si>
+  <si>
+    <t>obtidas através dos autovetores</t>
+  </si>
+  <si>
+    <t>Trata-se de técnica exploratória (não supervisionada)
+• Para avaliar a relação conjunta entre as variáveis (interdependência)
+• Não há modelos do tipo “yi = x1i + x2i + ... + ui”
+• Não são adequadas para fins de inferência
+• Se novas observações forem adicionadas ao banco de dados, é adequado refazer a análise</t>
+  </si>
+  <si>
+    <t>Tabela de resíduos padronizados ajustados
+• Se o valor do resíduo padronizado ajustado em certa célula for maior do que 1,96, interpreta-se que existe associação significativa, ao nível de significância de 5%, entre as duas categorias que interagem na célula; se for menor do que 1,96, não há associação estatisticamente significativa
+• 1,96 é o valor crítico da normal padrão para o nível de significância de 5%</t>
+  </si>
+  <si>
+    <t>As coordenadas das observações podem ser utilizadas como variaveis métricas, sem usar ponderação arbitrária. Pode ser usado onde as metricas são usadas</t>
+  </si>
+  <si>
+    <t>Não supervisionado</t>
+  </si>
+  <si>
+    <t>Clustering</t>
+  </si>
+  <si>
+    <t>agrupar as observações em grupos homogêneos
+internamente e heterogêneos entre si</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Uso</t>
+  </si>
+  <si>
+    <t>Método Não Hierárquico K-means
+• Define-se a priori quantos cluster serão formados</t>
+  </si>
+  <si>
+    <t>Técnicas</t>
+  </si>
+  <si>
+    <t>Análise Resultados</t>
+  </si>
+  <si>
+    <t>Observações</t>
+  </si>
+  <si>
+    <t>Análise de Correspondencia Simples e Múltipla (Anacor e MCA)</t>
+  </si>
+  <si>
+    <t>SNA - Análise de Redes Sociais</t>
+  </si>
+  <si>
+    <t>tomada de decisão multicritério - AHP, ANP, PrOPPAGA, THOR, SAPEVO e TOPSIS.</t>
+  </si>
+  <si>
+    <t>Supervisionado</t>
+  </si>
+  <si>
+    <t>pode ser aplicado em amostras maiores</t>
+  </si>
+  <si>
+    <r>
+      <t>importante comparar se a variabilidade dentro do grupo é menor do que a variabilidade entre grupos. Usar o</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TESTE F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Método Hierárquico Aglomerativo
+• A quantidade de clusters é definida ao longo da análise</t>
+  </si>
+  <si>
+    <t>Técnica exploratória, não tem caráter preditivo para observações de fora da amostra</t>
+  </si>
+  <si>
+    <t>Análise Componentes Principais (PCA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+agrupar as variáveis em fatores</t>
+  </si>
+  <si>
+    <t>Sensível à presença de outliers
+Para variáveis categóricas, pode usar a Análise de Correspondência</t>
+  </si>
+  <si>
+    <t>Técnica exploratória, não tem caráter preditivo para observações de fora da amostra. 
+Redução de dimensionalidade</t>
+  </si>
+  <si>
+    <t>Para investigar a adequação global da análise fatorial usa-se o teste de esfericidade de Bartlett</t>
+  </si>
+  <si>
+    <t>Análise de variáveis categóricas</t>
+  </si>
+  <si>
+    <t>Verificar se existe associação estatisticamente significativa entre as variáveis e suas categorias</t>
+  </si>
+  <si>
+    <t>Para Variáveis categóricas. 
+Variável quantitativa deve passar por um processo de categorização previamente
+Pode ser usado para transformar categórica em métrica sem usar ponderação arbitrária.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1007,16 +1169,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1039,12 +1214,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1077,6 +1290,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1092,13 +1317,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="2" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1114,6 +1352,130 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>706144</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>67376</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Agrupar 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E06469C7-8C20-649E-E0F6-8185C6930BAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9659644" cy="5020376"/>
+          <a:chOff x="0" y="0"/>
+          <a:chExt cx="9269119" cy="5020376"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="2" name="Imagem 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA71EA81-25F1-244F-E3BF-B7A8C1CFADF6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="9269119" cy="5020376"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="CaixaDeTexto 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAC655EE-05E6-E74B-B885-274CE94FBD96}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2247900" y="209550"/>
+            <a:ext cx="3962400" cy="295275"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1100" b="1" i="1"/>
+              <a:t>https://scikit-learn.org/stable/machine_learning_map</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1294,7 +1656,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1387,7 +1749,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1436,7 +1798,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1755,28 +2117,288 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296FDF35-1B9F-4DAC-B2B5-48FAD05CE690}">
-  <dimension ref="C2:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36DF5BCB-606A-4DB5-8AD0-638D34003BD4}">
+  <dimension ref="A28:G46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="41.140625" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>67</v>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="26"/>
+      <c r="B31" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="26"/>
+      <c r="B32" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="27"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="26"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="6"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="26"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="26"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="27"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="6"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="A34:A38"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="B2:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="78" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1784,7 +2406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="I2:I3"/>
   <sheetViews>
@@ -1815,6 +2437,391 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:V28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="19"/>
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="19"/>
+      <c r="C11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12" s="19"/>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+    </row>
+    <row r="14" spans="2:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="19"/>
+      <c r="C14" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="19"/>
+      <c r="C15" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="18"/>
+      <c r="C24" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="18"/>
+      <c r="C25" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B27" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="B28" s="18"/>
+      <c r="C28" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="O6:V6"/>
+    <mergeCell ref="F13:M13"/>
+    <mergeCell ref="B13:B15"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9065BC9-6437-4A90-8675-040CA624184B}">
+  <dimension ref="B2:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="3" max="3" width="94.5703125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="21"/>
+      <c r="C9" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B8:B9"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CB75A2-2512-40A0-8BED-9933E8A0C9BA}">
+  <dimension ref="B2:D14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="59.28515625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="71" style="15" customWidth="1"/>
+    <col min="4" max="4" width="66" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="17">
+        <f>23000*0.275*12</f>
+        <v>75900.000000000015</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C9" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D15"/>
   <sheetViews>
@@ -1933,15 +2940,15 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C15" s="10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1953,304 +2960,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:V28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="2:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="2:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="2:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="2:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-    </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="2:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
-      <c r="C10" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="2:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
-      <c r="C11" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="2:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
-      <c r="C12" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="2:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-    </row>
-    <row r="14" spans="2:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="15"/>
-      <c r="C14" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="2:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="15"/>
-      <c r="C15" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="14"/>
-      <c r="C24" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="14"/>
-      <c r="C25" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B27" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" ht="195" x14ac:dyDescent="0.25">
-      <c r="B28" s="14"/>
-      <c r="C28" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="G6:M6"/>
-    <mergeCell ref="O6:V6"/>
-    <mergeCell ref="F13:M13"/>
-    <mergeCell ref="B13:B15"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9065BC9-6437-4A90-8675-040CA624184B}">
-  <dimension ref="B2:C13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="50" customWidth="1"/>
-    <col min="3" max="3" width="94.5703125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
-      <c r="C9" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B8:B9"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -2308,12 +3022,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5B6F93-226F-4C47-80C8-E595635592CA}">
   <dimension ref="B2:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2327,23 +3041,23 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2351,7 +3065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:C2"/>
   <sheetViews>
@@ -2374,12 +3088,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2394,7 +3108,7 @@
       </c>
     </row>
     <row r="4" spans="2:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="19" t="s">
         <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -2402,13 +3116,13 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="22" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2416,22 +3130,22 @@
       </c>
     </row>
     <row r="7" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="18"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="18"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="18"/>
+      <c r="B9" s="22"/>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="22" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -2439,19 +3153,19 @@
       </c>
     </row>
     <row r="11" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="18"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="18"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -2459,7 +3173,7 @@
       </c>
     </row>
     <row r="15" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="18"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="1" t="s">
         <v>48</v>
       </c>
@@ -2474,39 +3188,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B2:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="25.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="78" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>